<commit_message>
fix model, fix tests
</commit_message>
<xml_diff>
--- a/bbgraph-init/src/main/resources/init/business_data.xlsx
+++ b/bbgraph-init/src/main/resources/init/business_data.xlsx
@@ -281,7 +281,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -352,7 +352,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -430,13 +430,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
@@ -525,17 +525,17 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
@@ -600,6 +600,13 @@
         <v>22</v>
       </c>
     </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
import: fix empty lines
</commit_message>
<xml_diff>
--- a/bbgraph-init/src/main/resources/init/business_data.xlsx
+++ b/bbgraph-init/src/main/resources/init/business_data.xlsx
@@ -253,23 +253,6 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:I2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I2"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="firstName"/>
-    <tableColumn id="3" name="lastName"/>
-    <tableColumn id="4" name="username"/>
-    <tableColumn id="5" name="email"/>
-    <tableColumn id="6" name="password"/>
-    <tableColumn id="7" name="groups"/>
-    <tableColumn id="8" name="authorities"/>
-    <tableColumn id="9" name="locale"/>
-  </tableColumns>
-</table>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -281,7 +264,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -352,7 +335,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -430,7 +413,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.02"/>
@@ -522,27 +505,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="10" style="0" width="10.29"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,19 +571,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="lalmeras@gmail.com"/>
@@ -624,8 +582,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>